<commit_message>
updated my project source code
</commit_message>
<xml_diff>
--- a/testdata/Opencart_LoginData.xlsx
+++ b/testdata/Opencart_LoginData.xlsx
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Start123</t>
+  </si>
+  <si>
+    <t>Binduraj@24</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="E5" sqref="E5" activeCellId="0"/>
+      <selection activeCell="C4" sqref="C4" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -571,7 +574,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>

</xml_diff>